<commit_message>
SED-4528 improving Junit tests
</commit_message>
<xml_diff>
--- a/step-automation-packages/step-automation-packages-samples/step-automation-packages-sample2/src/main/resources/excel/excel1.xlsx
+++ b/step-automation-packages/step-automation-packages-samples/step-automation-packages-sample2/src/main/resources/excel/excel1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="myWorksheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="myWorksheet" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -19,6 +19,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col1_Row1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col2_Row1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col1_Row2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col2_Row2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -35,19 +58,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,25 +129,156 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SED-4528 ap dataset with files cannot be created in a before sections (#593)
* SED-4528 AP - dataset with files cannot be created in a before sections

* SED-4528 improving Junit tests

* SED-4528 PR feedbacks

* SED-4546 Auto-Provisioning - Execution does not timeout after the agents failed to start

* Revert "SED-4546 Auto-Provisioning - Execution does not timeout after the agents failed to start"

This reverts commit 1a032862a7a1182ff7a020195c1f0e689dfcdbd4.
</commit_message>
<xml_diff>
--- a/step-automation-packages/step-automation-packages-samples/step-automation-packages-sample2/src/main/resources/excel/excel1.xlsx
+++ b/step-automation-packages/step-automation-packages-samples/step-automation-packages-sample2/src/main/resources/excel/excel1.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="myWorksheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="myWorksheet" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -19,6 +19,29 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">Col1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Col2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col1_Row1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col2_Row1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col1_Row2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val_Col2_Row2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -35,19 +58,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,25 +129,156 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>